<commit_message>
excel data provider completed
</commit_message>
<xml_diff>
--- a/DevStackAutomationFramework/src/test/resources/excelData/LoginTest.xlsx
+++ b/DevStackAutomationFramework/src/test/resources/excelData/LoginTest.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thameeramalinga/DeveloperStackQA/Framework/DevStackAutomationFramework/DevStackAutomationFramework/src/test/resources/excelData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AF6199C-7E73-FE47-9D57-D516A68E8BA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5075EC9D-11F8-674B-BE21-13D1C8E09F58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="1800" windowWidth="28040" windowHeight="17440" xr2:uid="{1BC3C561-4519-DC4B-97F5-0E0D12BD283E}"/>
+    <workbookView xWindow="4940" yWindow="2440" windowWidth="28040" windowHeight="17440" xr2:uid="{1BC3C561-4519-DC4B-97F5-0E0D12BD283E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="loginTest" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>

</xml_diff>